<commit_message>
Fix the scenario analysis
Instances have to be generated seperately. There are some things left in memory!!
</commit_message>
<xml_diff>
--- a/Output/results.xlsx
+++ b/Output/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -645,7 +645,6 @@
           <t>27/04/2022 17:31:55</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
       <c r="C6" t="n">
         <v>7</v>
       </c>
@@ -664,18 +663,12 @@
       <c r="H6" t="n">
         <v>7</v>
       </c>
-      <c r="I6" t="inlineStr"/>
       <c r="J6" t="n">
         <v>17</v>
       </c>
       <c r="K6" t="n">
         <v>1</v>
       </c>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -683,7 +676,6 @@
           <t>27/04/2022 17:31:55</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
       <c r="C7" t="n">
         <v>8</v>
       </c>
@@ -702,18 +694,12 @@
       <c r="H7" t="n">
         <v>7</v>
       </c>
-      <c r="I7" t="inlineStr"/>
       <c r="J7" t="n">
         <v>30</v>
       </c>
       <c r="K7" t="n">
         <v>2</v>
       </c>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -721,7 +707,6 @@
           <t>27/04/2022 17:31:55</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr"/>
       <c r="C8" t="n">
         <v>9</v>
       </c>
@@ -740,18 +725,12 @@
       <c r="H8" t="n">
         <v>7</v>
       </c>
-      <c r="I8" t="inlineStr"/>
       <c r="J8" t="n">
         <v>36</v>
       </c>
       <c r="K8" t="n">
         <v>3</v>
       </c>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -759,7 +738,6 @@
           <t>27/04/2022 17:31:55</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
       <c r="C9" t="n">
         <v>10</v>
       </c>
@@ -778,18 +756,1900 @@
       <c r="H9" t="n">
         <v>7</v>
       </c>
-      <c r="I9" t="inlineStr"/>
       <c r="J9" t="n">
         <v>43</v>
       </c>
       <c r="K9" t="n">
         <v>3</v>
       </c>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:26:03</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>7</v>
+      </c>
+      <c r="D10" t="n">
+        <v>20</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3</v>
+      </c>
+      <c r="F10" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" t="n">
+        <v>25</v>
+      </c>
+      <c r="H10" t="n">
+        <v>7</v>
+      </c>
+      <c r="J10" t="n">
+        <v>14</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:26:03</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>8</v>
+      </c>
+      <c r="D11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3</v>
+      </c>
+      <c r="F11" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" t="n">
+        <v>25</v>
+      </c>
+      <c r="H11" t="n">
+        <v>7</v>
+      </c>
+      <c r="J11" t="n">
+        <v>22</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:26:03</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>9</v>
+      </c>
+      <c r="D12" t="n">
+        <v>20</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" t="n">
+        <v>25</v>
+      </c>
+      <c r="H12" t="n">
+        <v>7</v>
+      </c>
+      <c r="J12" t="n">
+        <v>23</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:26:03</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>10</v>
+      </c>
+      <c r="D13" t="n">
+        <v>20</v>
+      </c>
+      <c r="E13" t="n">
+        <v>3</v>
+      </c>
+      <c r="F13" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" t="n">
+        <v>25</v>
+      </c>
+      <c r="H13" t="n">
+        <v>7</v>
+      </c>
+      <c r="J13" t="n">
+        <v>27</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:26:03</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>7</v>
+      </c>
+      <c r="D14" t="n">
+        <v>20</v>
+      </c>
+      <c r="E14" t="n">
+        <v>5</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" t="n">
+        <v>25</v>
+      </c>
+      <c r="H14" t="n">
+        <v>7</v>
+      </c>
+      <c r="J14" t="n">
+        <v>14</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:26:03</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>8</v>
+      </c>
+      <c r="D15" t="n">
+        <v>20</v>
+      </c>
+      <c r="E15" t="n">
+        <v>5</v>
+      </c>
+      <c r="F15" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" t="n">
+        <v>25</v>
+      </c>
+      <c r="H15" t="n">
+        <v>7</v>
+      </c>
+      <c r="J15" t="n">
+        <v>20</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:26:03</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>9</v>
+      </c>
+      <c r="D16" t="n">
+        <v>20</v>
+      </c>
+      <c r="E16" t="n">
+        <v>5</v>
+      </c>
+      <c r="F16" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" t="n">
+        <v>25</v>
+      </c>
+      <c r="H16" t="n">
+        <v>7</v>
+      </c>
+      <c r="J16" t="n">
+        <v>23</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:26:03</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>10</v>
+      </c>
+      <c r="D17" t="n">
+        <v>20</v>
+      </c>
+      <c r="E17" t="n">
+        <v>5</v>
+      </c>
+      <c r="F17" t="n">
+        <v>2</v>
+      </c>
+      <c r="G17" t="n">
+        <v>25</v>
+      </c>
+      <c r="H17" t="n">
+        <v>7</v>
+      </c>
+      <c r="J17" t="n">
+        <v>26</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:30:20</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>7</v>
+      </c>
+      <c r="D18" t="n">
+        <v>50</v>
+      </c>
+      <c r="E18" t="n">
+        <v>3</v>
+      </c>
+      <c r="F18" t="n">
+        <v>2</v>
+      </c>
+      <c r="G18" t="n">
+        <v>25</v>
+      </c>
+      <c r="H18" t="n">
+        <v>7</v>
+      </c>
+      <c r="J18" t="n">
+        <v>156</v>
+      </c>
+      <c r="K18" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:30:20</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>8</v>
+      </c>
+      <c r="D19" t="n">
+        <v>50</v>
+      </c>
+      <c r="E19" t="n">
+        <v>3</v>
+      </c>
+      <c r="F19" t="n">
+        <v>2</v>
+      </c>
+      <c r="G19" t="n">
+        <v>25</v>
+      </c>
+      <c r="H19" t="n">
+        <v>7</v>
+      </c>
+      <c r="J19" t="n">
+        <v>272</v>
+      </c>
+      <c r="K19" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:30:20</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>9</v>
+      </c>
+      <c r="D20" t="n">
+        <v>50</v>
+      </c>
+      <c r="E20" t="n">
+        <v>3</v>
+      </c>
+      <c r="F20" t="n">
+        <v>2</v>
+      </c>
+      <c r="G20" t="n">
+        <v>25</v>
+      </c>
+      <c r="H20" t="n">
+        <v>7</v>
+      </c>
+      <c r="J20" t="n">
+        <v>316</v>
+      </c>
+      <c r="K20" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:30:20</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>10</v>
+      </c>
+      <c r="D21" t="n">
+        <v>50</v>
+      </c>
+      <c r="E21" t="n">
+        <v>3</v>
+      </c>
+      <c r="F21" t="n">
+        <v>2</v>
+      </c>
+      <c r="G21" t="n">
+        <v>25</v>
+      </c>
+      <c r="H21" t="n">
+        <v>7</v>
+      </c>
+      <c r="J21" t="n">
+        <v>359</v>
+      </c>
+      <c r="K21" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:37:35</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>7</v>
+      </c>
+      <c r="D22" t="n">
+        <v>50</v>
+      </c>
+      <c r="E22" t="n">
+        <v>3</v>
+      </c>
+      <c r="F22" t="n">
+        <v>2</v>
+      </c>
+      <c r="G22" t="n">
+        <v>25</v>
+      </c>
+      <c r="H22" t="n">
+        <v>7</v>
+      </c>
+      <c r="J22" t="n">
+        <v>152</v>
+      </c>
+      <c r="K22" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:37:35</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>8</v>
+      </c>
+      <c r="D23" t="n">
+        <v>50</v>
+      </c>
+      <c r="E23" t="n">
+        <v>3</v>
+      </c>
+      <c r="F23" t="n">
+        <v>2</v>
+      </c>
+      <c r="G23" t="n">
+        <v>25</v>
+      </c>
+      <c r="H23" t="n">
+        <v>7</v>
+      </c>
+      <c r="J23" t="n">
+        <v>277</v>
+      </c>
+      <c r="K23" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:37:35</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>9</v>
+      </c>
+      <c r="D24" t="n">
+        <v>50</v>
+      </c>
+      <c r="E24" t="n">
+        <v>3</v>
+      </c>
+      <c r="F24" t="n">
+        <v>2</v>
+      </c>
+      <c r="G24" t="n">
+        <v>25</v>
+      </c>
+      <c r="H24" t="n">
+        <v>7</v>
+      </c>
+      <c r="J24" t="n">
+        <v>324</v>
+      </c>
+      <c r="K24" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:37:35</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>10</v>
+      </c>
+      <c r="D25" t="n">
+        <v>50</v>
+      </c>
+      <c r="E25" t="n">
+        <v>3</v>
+      </c>
+      <c r="F25" t="n">
+        <v>2</v>
+      </c>
+      <c r="G25" t="n">
+        <v>25</v>
+      </c>
+      <c r="H25" t="n">
+        <v>7</v>
+      </c>
+      <c r="J25" t="n">
+        <v>355</v>
+      </c>
+      <c r="K25" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:39:04</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>7</v>
+      </c>
+      <c r="D26" t="n">
+        <v>50</v>
+      </c>
+      <c r="E26" t="n">
+        <v>3</v>
+      </c>
+      <c r="F26" t="n">
+        <v>2</v>
+      </c>
+      <c r="G26" t="n">
+        <v>25</v>
+      </c>
+      <c r="H26" t="n">
+        <v>7</v>
+      </c>
+      <c r="J26" t="n">
+        <v>152</v>
+      </c>
+      <c r="K26" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:39:04</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>8</v>
+      </c>
+      <c r="D27" t="n">
+        <v>50</v>
+      </c>
+      <c r="E27" t="n">
+        <v>3</v>
+      </c>
+      <c r="F27" t="n">
+        <v>2</v>
+      </c>
+      <c r="G27" t="n">
+        <v>25</v>
+      </c>
+      <c r="H27" t="n">
+        <v>7</v>
+      </c>
+      <c r="J27" t="n">
+        <v>277</v>
+      </c>
+      <c r="K27" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:39:04</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>9</v>
+      </c>
+      <c r="D28" t="n">
+        <v>50</v>
+      </c>
+      <c r="E28" t="n">
+        <v>3</v>
+      </c>
+      <c r="F28" t="n">
+        <v>2</v>
+      </c>
+      <c r="G28" t="n">
+        <v>25</v>
+      </c>
+      <c r="H28" t="n">
+        <v>7</v>
+      </c>
+      <c r="J28" t="n">
+        <v>324</v>
+      </c>
+      <c r="K28" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:39:04</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>10</v>
+      </c>
+      <c r="D29" t="n">
+        <v>50</v>
+      </c>
+      <c r="E29" t="n">
+        <v>3</v>
+      </c>
+      <c r="F29" t="n">
+        <v>2</v>
+      </c>
+      <c r="G29" t="n">
+        <v>25</v>
+      </c>
+      <c r="H29" t="n">
+        <v>7</v>
+      </c>
+      <c r="J29" t="n">
+        <v>355</v>
+      </c>
+      <c r="K29" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:39:42</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>7</v>
+      </c>
+      <c r="D30" t="n">
+        <v>50</v>
+      </c>
+      <c r="E30" t="n">
+        <v>3</v>
+      </c>
+      <c r="F30" t="n">
+        <v>2</v>
+      </c>
+      <c r="G30" t="n">
+        <v>25</v>
+      </c>
+      <c r="H30" t="n">
+        <v>7</v>
+      </c>
+      <c r="J30" t="n">
+        <v>152</v>
+      </c>
+      <c r="K30" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:39:42</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>8</v>
+      </c>
+      <c r="D31" t="n">
+        <v>50</v>
+      </c>
+      <c r="E31" t="n">
+        <v>3</v>
+      </c>
+      <c r="F31" t="n">
+        <v>2</v>
+      </c>
+      <c r="G31" t="n">
+        <v>25</v>
+      </c>
+      <c r="H31" t="n">
+        <v>7</v>
+      </c>
+      <c r="J31" t="n">
+        <v>277</v>
+      </c>
+      <c r="K31" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:39:42</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>9</v>
+      </c>
+      <c r="D32" t="n">
+        <v>50</v>
+      </c>
+      <c r="E32" t="n">
+        <v>3</v>
+      </c>
+      <c r="F32" t="n">
+        <v>2</v>
+      </c>
+      <c r="G32" t="n">
+        <v>25</v>
+      </c>
+      <c r="H32" t="n">
+        <v>7</v>
+      </c>
+      <c r="J32" t="n">
+        <v>324</v>
+      </c>
+      <c r="K32" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:39:42</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>10</v>
+      </c>
+      <c r="D33" t="n">
+        <v>50</v>
+      </c>
+      <c r="E33" t="n">
+        <v>3</v>
+      </c>
+      <c r="F33" t="n">
+        <v>2</v>
+      </c>
+      <c r="G33" t="n">
+        <v>25</v>
+      </c>
+      <c r="H33" t="n">
+        <v>7</v>
+      </c>
+      <c r="J33" t="n">
+        <v>355</v>
+      </c>
+      <c r="K33" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:40:14</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>7</v>
+      </c>
+      <c r="D34" t="n">
+        <v>50</v>
+      </c>
+      <c r="E34" t="n">
+        <v>3</v>
+      </c>
+      <c r="F34" t="n">
+        <v>2</v>
+      </c>
+      <c r="G34" t="n">
+        <v>25</v>
+      </c>
+      <c r="H34" t="n">
+        <v>7</v>
+      </c>
+      <c r="J34" t="n">
+        <v>152</v>
+      </c>
+      <c r="K34" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:40:14</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>8</v>
+      </c>
+      <c r="D35" t="n">
+        <v>50</v>
+      </c>
+      <c r="E35" t="n">
+        <v>3</v>
+      </c>
+      <c r="F35" t="n">
+        <v>2</v>
+      </c>
+      <c r="G35" t="n">
+        <v>25</v>
+      </c>
+      <c r="H35" t="n">
+        <v>7</v>
+      </c>
+      <c r="J35" t="n">
+        <v>277</v>
+      </c>
+      <c r="K35" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:40:14</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>9</v>
+      </c>
+      <c r="D36" t="n">
+        <v>50</v>
+      </c>
+      <c r="E36" t="n">
+        <v>3</v>
+      </c>
+      <c r="F36" t="n">
+        <v>2</v>
+      </c>
+      <c r="G36" t="n">
+        <v>25</v>
+      </c>
+      <c r="H36" t="n">
+        <v>7</v>
+      </c>
+      <c r="J36" t="n">
+        <v>324</v>
+      </c>
+      <c r="K36" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:40:14</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>10</v>
+      </c>
+      <c r="D37" t="n">
+        <v>50</v>
+      </c>
+      <c r="E37" t="n">
+        <v>3</v>
+      </c>
+      <c r="F37" t="n">
+        <v>2</v>
+      </c>
+      <c r="G37" t="n">
+        <v>25</v>
+      </c>
+      <c r="H37" t="n">
+        <v>7</v>
+      </c>
+      <c r="J37" t="n">
+        <v>355</v>
+      </c>
+      <c r="K37" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:41:23</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>7</v>
+      </c>
+      <c r="D38" t="n">
+        <v>50</v>
+      </c>
+      <c r="E38" t="n">
+        <v>3</v>
+      </c>
+      <c r="F38" t="n">
+        <v>2</v>
+      </c>
+      <c r="G38" t="n">
+        <v>25</v>
+      </c>
+      <c r="H38" t="n">
+        <v>7</v>
+      </c>
+      <c r="J38" t="n">
+        <v>152</v>
+      </c>
+      <c r="K38" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:41:23</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>8</v>
+      </c>
+      <c r="D39" t="n">
+        <v>50</v>
+      </c>
+      <c r="E39" t="n">
+        <v>3</v>
+      </c>
+      <c r="F39" t="n">
+        <v>2</v>
+      </c>
+      <c r="G39" t="n">
+        <v>25</v>
+      </c>
+      <c r="H39" t="n">
+        <v>7</v>
+      </c>
+      <c r="J39" t="n">
+        <v>277</v>
+      </c>
+      <c r="K39" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:41:23</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>9</v>
+      </c>
+      <c r="D40" t="n">
+        <v>50</v>
+      </c>
+      <c r="E40" t="n">
+        <v>3</v>
+      </c>
+      <c r="F40" t="n">
+        <v>2</v>
+      </c>
+      <c r="G40" t="n">
+        <v>25</v>
+      </c>
+      <c r="H40" t="n">
+        <v>7</v>
+      </c>
+      <c r="J40" t="n">
+        <v>324</v>
+      </c>
+      <c r="K40" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:41:23</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>10</v>
+      </c>
+      <c r="D41" t="n">
+        <v>50</v>
+      </c>
+      <c r="E41" t="n">
+        <v>3</v>
+      </c>
+      <c r="F41" t="n">
+        <v>2</v>
+      </c>
+      <c r="G41" t="n">
+        <v>25</v>
+      </c>
+      <c r="H41" t="n">
+        <v>7</v>
+      </c>
+      <c r="J41" t="n">
+        <v>355</v>
+      </c>
+      <c r="K41" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:50:26</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>7</v>
+      </c>
+      <c r="D42" t="n">
+        <v>50</v>
+      </c>
+      <c r="E42" t="n">
+        <v>3</v>
+      </c>
+      <c r="F42" t="n">
+        <v>2</v>
+      </c>
+      <c r="G42" t="n">
+        <v>25</v>
+      </c>
+      <c r="H42" t="n">
+        <v>7</v>
+      </c>
+      <c r="J42" t="n">
+        <v>152</v>
+      </c>
+      <c r="K42" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:50:26</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>8</v>
+      </c>
+      <c r="D43" t="n">
+        <v>50</v>
+      </c>
+      <c r="E43" t="n">
+        <v>3</v>
+      </c>
+      <c r="F43" t="n">
+        <v>2</v>
+      </c>
+      <c r="G43" t="n">
+        <v>25</v>
+      </c>
+      <c r="H43" t="n">
+        <v>7</v>
+      </c>
+      <c r="J43" t="n">
+        <v>277</v>
+      </c>
+      <c r="K43" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:50:26</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>9</v>
+      </c>
+      <c r="D44" t="n">
+        <v>50</v>
+      </c>
+      <c r="E44" t="n">
+        <v>3</v>
+      </c>
+      <c r="F44" t="n">
+        <v>2</v>
+      </c>
+      <c r="G44" t="n">
+        <v>25</v>
+      </c>
+      <c r="H44" t="n">
+        <v>7</v>
+      </c>
+      <c r="J44" t="n">
+        <v>324</v>
+      </c>
+      <c r="K44" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:50:26</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>10</v>
+      </c>
+      <c r="D45" t="n">
+        <v>50</v>
+      </c>
+      <c r="E45" t="n">
+        <v>3</v>
+      </c>
+      <c r="F45" t="n">
+        <v>2</v>
+      </c>
+      <c r="G45" t="n">
+        <v>25</v>
+      </c>
+      <c r="H45" t="n">
+        <v>7</v>
+      </c>
+      <c r="J45" t="n">
+        <v>355</v>
+      </c>
+      <c r="K45" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:51:55</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>7</v>
+      </c>
+      <c r="D46" t="n">
+        <v>50</v>
+      </c>
+      <c r="E46" t="n">
+        <v>3</v>
+      </c>
+      <c r="F46" t="n">
+        <v>2</v>
+      </c>
+      <c r="G46" t="n">
+        <v>25</v>
+      </c>
+      <c r="H46" t="n">
+        <v>7</v>
+      </c>
+      <c r="J46" t="n">
+        <v>156</v>
+      </c>
+      <c r="K46" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:51:55</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>8</v>
+      </c>
+      <c r="D47" t="n">
+        <v>50</v>
+      </c>
+      <c r="E47" t="n">
+        <v>3</v>
+      </c>
+      <c r="F47" t="n">
+        <v>2</v>
+      </c>
+      <c r="G47" t="n">
+        <v>25</v>
+      </c>
+      <c r="H47" t="n">
+        <v>7</v>
+      </c>
+      <c r="J47" t="n">
+        <v>272</v>
+      </c>
+      <c r="K47" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:51:55</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>9</v>
+      </c>
+      <c r="D48" t="n">
+        <v>50</v>
+      </c>
+      <c r="E48" t="n">
+        <v>3</v>
+      </c>
+      <c r="F48" t="n">
+        <v>2</v>
+      </c>
+      <c r="G48" t="n">
+        <v>25</v>
+      </c>
+      <c r="H48" t="n">
+        <v>7</v>
+      </c>
+      <c r="J48" t="n">
+        <v>316</v>
+      </c>
+      <c r="K48" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:51:55</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>10</v>
+      </c>
+      <c r="D49" t="n">
+        <v>50</v>
+      </c>
+      <c r="E49" t="n">
+        <v>3</v>
+      </c>
+      <c r="F49" t="n">
+        <v>2</v>
+      </c>
+      <c r="G49" t="n">
+        <v>25</v>
+      </c>
+      <c r="H49" t="n">
+        <v>7</v>
+      </c>
+      <c r="J49" t="n">
+        <v>359</v>
+      </c>
+      <c r="K49" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:52:43</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>7</v>
+      </c>
+      <c r="D50" t="n">
+        <v>50</v>
+      </c>
+      <c r="E50" t="n">
+        <v>3</v>
+      </c>
+      <c r="F50" t="n">
+        <v>2</v>
+      </c>
+      <c r="G50" t="n">
+        <v>25</v>
+      </c>
+      <c r="H50" t="n">
+        <v>7</v>
+      </c>
+      <c r="J50" t="n">
+        <v>156</v>
+      </c>
+      <c r="K50" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:52:43</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>8</v>
+      </c>
+      <c r="D51" t="n">
+        <v>50</v>
+      </c>
+      <c r="E51" t="n">
+        <v>3</v>
+      </c>
+      <c r="F51" t="n">
+        <v>2</v>
+      </c>
+      <c r="G51" t="n">
+        <v>25</v>
+      </c>
+      <c r="H51" t="n">
+        <v>7</v>
+      </c>
+      <c r="J51" t="n">
+        <v>272</v>
+      </c>
+      <c r="K51" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:52:43</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>9</v>
+      </c>
+      <c r="D52" t="n">
+        <v>50</v>
+      </c>
+      <c r="E52" t="n">
+        <v>3</v>
+      </c>
+      <c r="F52" t="n">
+        <v>2</v>
+      </c>
+      <c r="G52" t="n">
+        <v>25</v>
+      </c>
+      <c r="H52" t="n">
+        <v>7</v>
+      </c>
+      <c r="J52" t="n">
+        <v>316</v>
+      </c>
+      <c r="K52" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>28/04/2022 09:52:43</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>10</v>
+      </c>
+      <c r="D53" t="n">
+        <v>50</v>
+      </c>
+      <c r="E53" t="n">
+        <v>3</v>
+      </c>
+      <c r="F53" t="n">
+        <v>2</v>
+      </c>
+      <c r="G53" t="n">
+        <v>25</v>
+      </c>
+      <c r="H53" t="n">
+        <v>7</v>
+      </c>
+      <c r="J53" t="n">
+        <v>359</v>
+      </c>
+      <c r="K53" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>28/04/2022 10:01:26</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>7</v>
+      </c>
+      <c r="D54" t="n">
+        <v>50</v>
+      </c>
+      <c r="E54" t="n">
+        <v>3</v>
+      </c>
+      <c r="F54" t="n">
+        <v>2</v>
+      </c>
+      <c r="G54" t="n">
+        <v>25</v>
+      </c>
+      <c r="H54" t="n">
+        <v>7</v>
+      </c>
+      <c r="J54" t="n">
+        <v>156</v>
+      </c>
+      <c r="K54" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>28/04/2022 10:01:26</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>8</v>
+      </c>
+      <c r="D55" t="n">
+        <v>50</v>
+      </c>
+      <c r="E55" t="n">
+        <v>3</v>
+      </c>
+      <c r="F55" t="n">
+        <v>2</v>
+      </c>
+      <c r="G55" t="n">
+        <v>25</v>
+      </c>
+      <c r="H55" t="n">
+        <v>7</v>
+      </c>
+      <c r="J55" t="n">
+        <v>272</v>
+      </c>
+      <c r="K55" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>28/04/2022 10:01:26</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>9</v>
+      </c>
+      <c r="D56" t="n">
+        <v>50</v>
+      </c>
+      <c r="E56" t="n">
+        <v>3</v>
+      </c>
+      <c r="F56" t="n">
+        <v>2</v>
+      </c>
+      <c r="G56" t="n">
+        <v>25</v>
+      </c>
+      <c r="H56" t="n">
+        <v>7</v>
+      </c>
+      <c r="J56" t="n">
+        <v>316</v>
+      </c>
+      <c r="K56" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>28/04/2022 10:01:26</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>10</v>
+      </c>
+      <c r="D57" t="n">
+        <v>50</v>
+      </c>
+      <c r="E57" t="n">
+        <v>3</v>
+      </c>
+      <c r="F57" t="n">
+        <v>2</v>
+      </c>
+      <c r="G57" t="n">
+        <v>25</v>
+      </c>
+      <c r="H57" t="n">
+        <v>7</v>
+      </c>
+      <c r="J57" t="n">
+        <v>359</v>
+      </c>
+      <c r="K57" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>28/04/2022 10:01:26</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>7</v>
+      </c>
+      <c r="D58" t="n">
+        <v>50</v>
+      </c>
+      <c r="E58" t="n">
+        <v>3</v>
+      </c>
+      <c r="F58" t="n">
+        <v>2</v>
+      </c>
+      <c r="G58" t="n">
+        <v>25</v>
+      </c>
+      <c r="H58" t="n">
+        <v>7</v>
+      </c>
+      <c r="J58" t="n">
+        <v>156</v>
+      </c>
+      <c r="K58" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>28/04/2022 10:01:26</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>8</v>
+      </c>
+      <c r="D59" t="n">
+        <v>50</v>
+      </c>
+      <c r="E59" t="n">
+        <v>3</v>
+      </c>
+      <c r="F59" t="n">
+        <v>2</v>
+      </c>
+      <c r="G59" t="n">
+        <v>25</v>
+      </c>
+      <c r="H59" t="n">
+        <v>7</v>
+      </c>
+      <c r="J59" t="n">
+        <v>272</v>
+      </c>
+      <c r="K59" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>28/04/2022 10:01:26</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>9</v>
+      </c>
+      <c r="D60" t="n">
+        <v>50</v>
+      </c>
+      <c r="E60" t="n">
+        <v>3</v>
+      </c>
+      <c r="F60" t="n">
+        <v>2</v>
+      </c>
+      <c r="G60" t="n">
+        <v>25</v>
+      </c>
+      <c r="H60" t="n">
+        <v>7</v>
+      </c>
+      <c r="J60" t="n">
+        <v>316</v>
+      </c>
+      <c r="K60" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>28/04/2022 10:01:26</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>10</v>
+      </c>
+      <c r="D61" t="n">
+        <v>50</v>
+      </c>
+      <c r="E61" t="n">
+        <v>3</v>
+      </c>
+      <c r="F61" t="n">
+        <v>2</v>
+      </c>
+      <c r="G61" t="n">
+        <v>25</v>
+      </c>
+      <c r="H61" t="n">
+        <v>7</v>
+      </c>
+      <c r="J61" t="n">
+        <v>359</v>
+      </c>
+      <c r="K61" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>28/04/2022 10:01:26</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>7</v>
+      </c>
+      <c r="D62" t="n">
+        <v>50</v>
+      </c>
+      <c r="E62" t="n">
+        <v>3</v>
+      </c>
+      <c r="F62" t="n">
+        <v>2</v>
+      </c>
+      <c r="G62" t="n">
+        <v>25</v>
+      </c>
+      <c r="H62" t="n">
+        <v>7</v>
+      </c>
+      <c r="J62" t="n">
+        <v>156</v>
+      </c>
+      <c r="K62" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>28/04/2022 10:01:26</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>8</v>
+      </c>
+      <c r="D63" t="n">
+        <v>50</v>
+      </c>
+      <c r="E63" t="n">
+        <v>3</v>
+      </c>
+      <c r="F63" t="n">
+        <v>2</v>
+      </c>
+      <c r="G63" t="n">
+        <v>25</v>
+      </c>
+      <c r="H63" t="n">
+        <v>7</v>
+      </c>
+      <c r="J63" t="n">
+        <v>272</v>
+      </c>
+      <c r="K63" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>28/04/2022 10:01:26</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>9</v>
+      </c>
+      <c r="D64" t="n">
+        <v>50</v>
+      </c>
+      <c r="E64" t="n">
+        <v>3</v>
+      </c>
+      <c r="F64" t="n">
+        <v>2</v>
+      </c>
+      <c r="G64" t="n">
+        <v>25</v>
+      </c>
+      <c r="H64" t="n">
+        <v>7</v>
+      </c>
+      <c r="J64" t="n">
+        <v>316</v>
+      </c>
+      <c r="K64" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>28/04/2022 10:01:26</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>10</v>
+      </c>
+      <c r="D65" t="n">
+        <v>50</v>
+      </c>
+      <c r="E65" t="n">
+        <v>3</v>
+      </c>
+      <c r="F65" t="n">
+        <v>2</v>
+      </c>
+      <c r="G65" t="n">
+        <v>25</v>
+      </c>
+      <c r="H65" t="n">
+        <v>7</v>
+      </c>
+      <c r="J65" t="n">
+        <v>359</v>
+      </c>
+      <c r="K65" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>28/04/2022 10:01:26</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr"/>
+      <c r="C66" t="n">
+        <v>7</v>
+      </c>
+      <c r="D66" t="n">
+        <v>50</v>
+      </c>
+      <c r="E66" t="n">
+        <v>3</v>
+      </c>
+      <c r="F66" t="n">
+        <v>2</v>
+      </c>
+      <c r="G66" t="n">
+        <v>25</v>
+      </c>
+      <c r="H66" t="n">
+        <v>7</v>
+      </c>
+      <c r="I66" t="inlineStr"/>
+      <c r="J66" t="n">
+        <v>156</v>
+      </c>
+      <c r="K66" t="n">
+        <v>11</v>
+      </c>
+      <c r="L66" t="inlineStr"/>
+      <c r="M66" t="inlineStr"/>
+      <c r="N66" t="inlineStr"/>
+      <c r="O66" t="inlineStr"/>
+      <c r="P66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>28/04/2022 10:01:26</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr"/>
+      <c r="C67" t="n">
+        <v>8</v>
+      </c>
+      <c r="D67" t="n">
+        <v>50</v>
+      </c>
+      <c r="E67" t="n">
+        <v>3</v>
+      </c>
+      <c r="F67" t="n">
+        <v>2</v>
+      </c>
+      <c r="G67" t="n">
+        <v>25</v>
+      </c>
+      <c r="H67" t="n">
+        <v>7</v>
+      </c>
+      <c r="I67" t="inlineStr"/>
+      <c r="J67" t="n">
+        <v>272</v>
+      </c>
+      <c r="K67" t="n">
+        <v>16</v>
+      </c>
+      <c r="L67" t="inlineStr"/>
+      <c r="M67" t="inlineStr"/>
+      <c r="N67" t="inlineStr"/>
+      <c r="O67" t="inlineStr"/>
+      <c r="P67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>28/04/2022 10:01:26</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr"/>
+      <c r="C68" t="n">
+        <v>9</v>
+      </c>
+      <c r="D68" t="n">
+        <v>50</v>
+      </c>
+      <c r="E68" t="n">
+        <v>3</v>
+      </c>
+      <c r="F68" t="n">
+        <v>2</v>
+      </c>
+      <c r="G68" t="n">
+        <v>25</v>
+      </c>
+      <c r="H68" t="n">
+        <v>7</v>
+      </c>
+      <c r="I68" t="inlineStr"/>
+      <c r="J68" t="n">
+        <v>316</v>
+      </c>
+      <c r="K68" t="n">
+        <v>24</v>
+      </c>
+      <c r="L68" t="inlineStr"/>
+      <c r="M68" t="inlineStr"/>
+      <c r="N68" t="inlineStr"/>
+      <c r="O68" t="inlineStr"/>
+      <c r="P68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>28/04/2022 10:01:26</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr"/>
+      <c r="C69" t="n">
+        <v>10</v>
+      </c>
+      <c r="D69" t="n">
+        <v>50</v>
+      </c>
+      <c r="E69" t="n">
+        <v>3</v>
+      </c>
+      <c r="F69" t="n">
+        <v>2</v>
+      </c>
+      <c r="G69" t="n">
+        <v>25</v>
+      </c>
+      <c r="H69" t="n">
+        <v>7</v>
+      </c>
+      <c r="I69" t="inlineStr"/>
+      <c r="J69" t="n">
+        <v>359</v>
+      </c>
+      <c r="K69" t="n">
+        <v>29</v>
+      </c>
+      <c r="L69" t="inlineStr"/>
+      <c r="M69" t="inlineStr"/>
+      <c r="N69" t="inlineStr"/>
+      <c r="O69" t="inlineStr"/>
+      <c r="P69" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>